<commit_message>
Modification de certaines tables à NULL dans le exel
</commit_message>
<xml_diff>
--- a/Documentation/TypeDesColonnesParTable.xlsx
+++ b/Documentation/TypeDesColonnesParTable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="4800" windowWidth="32860" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="-720" yWindow="100" windowWidth="25040" windowHeight="20180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1063,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A195" workbookViewId="0">
-      <selection activeCell="A240" sqref="A240:XFD241"/>
+    <sheetView tabSelected="1" topLeftCell="B35" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E230" sqref="E230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1936,7 +1936,7 @@
         <v>10</v>
       </c>
       <c r="E75">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -2062,7 +2062,7 @@
         <v>10</v>
       </c>
       <c r="E84">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -3671,7 +3671,7 @@
         <v>112</v>
       </c>
       <c r="D229" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="E229">
         <v>0</v>
@@ -3781,7 +3781,7 @@
         <v>10</v>
       </c>
       <c r="E238">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="239" spans="1:5">

</xml_diff>

<commit_message>
ajout isLike dans la table BLOG_like
</commit_message>
<xml_diff>
--- a/Documentation/TypeDesColonnesParTable.xlsx
+++ b/Documentation/TypeDesColonnesParTable.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="158">
   <si>
     <t>BLOG_Article</t>
   </si>
@@ -490,6 +490,9 @@
   </si>
   <si>
     <t>Valide</t>
+  </si>
+  <si>
+    <t>isLike</t>
   </si>
 </sst>
 </file>
@@ -1061,10 +1064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F240"/>
+  <dimension ref="A1:F241"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1550,34 +1553,34 @@
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="2" t="s">
+      <c r="B40" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" t="s">
+        <v>157</v>
+      </c>
+      <c r="D40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="3"/>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="B42" t="s">
-        <v>28</v>
-      </c>
-      <c r="C42" t="s">
-        <v>29</v>
-      </c>
-      <c r="D42" t="s">
-        <v>2</v>
-      </c>
-      <c r="E42">
-        <v>0</v>
-      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="3"/>
     </row>
     <row r="43" spans="1:5">
       <c r="B43" t="s">
         <v>28</v>
       </c>
       <c r="C43" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="D43" t="s">
         <v>2</v>
@@ -1591,10 +1594,10 @@
         <v>28</v>
       </c>
       <c r="C44" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D44" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -1605,7 +1608,7 @@
         <v>28</v>
       </c>
       <c r="C45" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D45" t="s">
         <v>31</v>
@@ -1619,47 +1622,47 @@
         <v>28</v>
       </c>
       <c r="C46" t="s">
+        <v>32</v>
+      </c>
+      <c r="D46" t="s">
+        <v>31</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="B47" t="s">
+        <v>28</v>
+      </c>
+      <c r="C47" t="s">
         <v>33</v>
       </c>
-      <c r="D46" t="s">
-        <v>5</v>
-      </c>
-      <c r="E46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="2" t="s">
+      <c r="D47" t="s">
+        <v>5</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="3"/>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="B49" t="s">
-        <v>34</v>
-      </c>
-      <c r="C49" t="s">
-        <v>19</v>
-      </c>
-      <c r="D49" t="s">
-        <v>2</v>
-      </c>
-      <c r="E49">
-        <v>0</v>
-      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="3"/>
     </row>
     <row r="50" spans="1:5">
       <c r="B50" t="s">
         <v>34</v>
       </c>
       <c r="C50" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="D50" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -1670,44 +1673,44 @@
         <v>34</v>
       </c>
       <c r="C51" t="s">
+        <v>35</v>
+      </c>
+      <c r="D51" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="B52" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" t="s">
         <v>6</v>
       </c>
-      <c r="D51" t="s">
-        <v>5</v>
-      </c>
-      <c r="E51">
+      <c r="D52" t="s">
+        <v>5</v>
+      </c>
+      <c r="E52">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="2" t="s">
+    <row r="53" spans="1:5">
+      <c r="A53" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="3"/>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="B54" t="s">
-        <v>36</v>
-      </c>
-      <c r="C54" t="s">
-        <v>37</v>
-      </c>
-      <c r="D54" t="s">
-        <v>2</v>
-      </c>
-      <c r="E54">
-        <v>0</v>
-      </c>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="3"/>
     </row>
     <row r="55" spans="1:5">
       <c r="B55" t="s">
         <v>36</v>
       </c>
       <c r="C55" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D55" t="s">
         <v>2</v>
@@ -1721,44 +1724,44 @@
         <v>36</v>
       </c>
       <c r="C56" t="s">
+        <v>38</v>
+      </c>
+      <c r="D56" t="s">
+        <v>2</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="B57" t="s">
+        <v>36</v>
+      </c>
+      <c r="C57" t="s">
         <v>15</v>
       </c>
-      <c r="D56" t="s">
-        <v>2</v>
-      </c>
-      <c r="E56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="2" t="s">
+      <c r="D57" t="s">
+        <v>2</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="3"/>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="B59" t="s">
-        <v>39</v>
-      </c>
-      <c r="C59" t="s">
-        <v>40</v>
-      </c>
-      <c r="D59" t="s">
-        <v>2</v>
-      </c>
-      <c r="E59">
-        <v>0</v>
-      </c>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="3"/>
     </row>
     <row r="60" spans="1:5">
       <c r="B60" t="s">
         <v>39</v>
       </c>
       <c r="C60" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="D60" t="s">
         <v>2</v>
@@ -1772,13 +1775,13 @@
         <v>39</v>
       </c>
       <c r="C61" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="D61" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E61">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1786,81 +1789,81 @@
         <v>39</v>
       </c>
       <c r="C62" t="s">
+        <v>41</v>
+      </c>
+      <c r="D62" t="s">
+        <v>5</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="B63" t="s">
+        <v>39</v>
+      </c>
+      <c r="C63" t="s">
         <v>42</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D63" t="s">
         <v>10</v>
       </c>
-      <c r="E62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="2" t="s">
+      <c r="E63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="3"/>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="B65" t="s">
-        <v>43</v>
-      </c>
-      <c r="C65" t="s">
-        <v>44</v>
-      </c>
-      <c r="D65" t="s">
-        <v>2</v>
-      </c>
-      <c r="E65">
-        <v>0</v>
-      </c>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="3"/>
     </row>
     <row r="66" spans="1:5">
       <c r="B66" t="s">
         <v>43</v>
       </c>
       <c r="C66" t="s">
+        <v>44</v>
+      </c>
+      <c r="D66" t="s">
+        <v>2</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="B67" t="s">
+        <v>43</v>
+      </c>
+      <c r="C67" t="s">
         <v>45</v>
       </c>
-      <c r="D66" t="s">
-        <v>5</v>
-      </c>
-      <c r="E66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" s="2" t="s">
+      <c r="D67" t="s">
+        <v>5</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="3"/>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="B69" t="s">
-        <v>46</v>
-      </c>
-      <c r="C69" t="s">
-        <v>8</v>
-      </c>
-      <c r="D69" t="s">
-        <v>2</v>
-      </c>
-      <c r="E69">
-        <v>0</v>
-      </c>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="3"/>
     </row>
     <row r="70" spans="1:5">
       <c r="B70" t="s">
         <v>46</v>
       </c>
       <c r="C70" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D70" t="s">
         <v>2</v>
@@ -1874,7 +1877,7 @@
         <v>46</v>
       </c>
       <c r="C71" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="D71" t="s">
         <v>2</v>
@@ -1888,7 +1891,7 @@
         <v>46</v>
       </c>
       <c r="C72" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="D72" t="s">
         <v>2</v>
@@ -1902,10 +1905,10 @@
         <v>46</v>
       </c>
       <c r="C73" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="D73" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E73">
         <v>0</v>
@@ -1916,7 +1919,7 @@
         <v>46</v>
       </c>
       <c r="C74" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="D74" t="s">
         <v>10</v>
@@ -1930,13 +1933,13 @@
         <v>46</v>
       </c>
       <c r="C75" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D75" t="s">
         <v>10</v>
       </c>
       <c r="E75">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -1944,13 +1947,13 @@
         <v>46</v>
       </c>
       <c r="C76" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="D76" t="s">
         <v>10</v>
       </c>
       <c r="E76">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -1958,10 +1961,10 @@
         <v>46</v>
       </c>
       <c r="C77" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D77" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E77">
         <v>0</v>
@@ -1972,13 +1975,13 @@
         <v>46</v>
       </c>
       <c r="C78" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D78" t="s">
         <v>5</v>
       </c>
       <c r="E78">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -1986,10 +1989,10 @@
         <v>46</v>
       </c>
       <c r="C79" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D79" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="E79">
         <v>1</v>
@@ -2000,7 +2003,7 @@
         <v>46</v>
       </c>
       <c r="C80" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D80" t="s">
         <v>31</v>
@@ -2014,10 +2017,10 @@
         <v>46</v>
       </c>
       <c r="C81" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D81" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="E81">
         <v>1</v>
@@ -2028,13 +2031,13 @@
         <v>46</v>
       </c>
       <c r="C82" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D82" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="E82">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -2042,10 +2045,10 @@
         <v>46</v>
       </c>
       <c r="C83" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D83" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="E83">
         <v>0</v>
@@ -2056,13 +2059,13 @@
         <v>46</v>
       </c>
       <c r="C84" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D84" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E84">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -2070,13 +2073,13 @@
         <v>46</v>
       </c>
       <c r="C85" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="D85" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E85">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -2084,44 +2087,44 @@
         <v>46</v>
       </c>
       <c r="C86" t="s">
+        <v>44</v>
+      </c>
+      <c r="D86" t="s">
+        <v>2</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="B87" t="s">
+        <v>46</v>
+      </c>
+      <c r="C87" t="s">
         <v>45</v>
       </c>
-      <c r="D86" t="s">
-        <v>5</v>
-      </c>
-      <c r="E86">
+      <c r="D87" t="s">
+        <v>5</v>
+      </c>
+      <c r="E87">
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
-      <c r="A87" s="2" t="s">
+    <row r="88" spans="1:5">
+      <c r="A88" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B87" s="2"/>
-      <c r="C87" s="2"/>
-      <c r="D87" s="2"/>
-      <c r="E87" s="3"/>
-    </row>
-    <row r="89" spans="1:5">
-      <c r="B89" t="s">
-        <v>59</v>
-      </c>
-      <c r="C89" t="s">
-        <v>60</v>
-      </c>
-      <c r="D89" t="s">
-        <v>2</v>
-      </c>
-      <c r="E89">
-        <v>0</v>
-      </c>
+      <c r="B88" s="2"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+      <c r="E88" s="3"/>
     </row>
     <row r="90" spans="1:5">
       <c r="B90" t="s">
         <v>59</v>
       </c>
       <c r="C90" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D90" t="s">
         <v>2</v>
@@ -2135,44 +2138,44 @@
         <v>59</v>
       </c>
       <c r="C91" t="s">
+        <v>8</v>
+      </c>
+      <c r="D91" t="s">
+        <v>2</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="B92" t="s">
+        <v>59</v>
+      </c>
+      <c r="C92" t="s">
         <v>61</v>
       </c>
-      <c r="D91" t="s">
-        <v>5</v>
-      </c>
-      <c r="E91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5">
-      <c r="A92" s="2" t="s">
+      <c r="D92" t="s">
+        <v>5</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
-      <c r="D92" s="2"/>
-      <c r="E92" s="3"/>
-    </row>
-    <row r="94" spans="1:5">
-      <c r="B94" t="s">
-        <v>62</v>
-      </c>
-      <c r="C94" t="s">
-        <v>63</v>
-      </c>
-      <c r="D94" t="s">
-        <v>2</v>
-      </c>
-      <c r="E94">
-        <v>0</v>
-      </c>
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
+      <c r="D93" s="2"/>
+      <c r="E93" s="3"/>
     </row>
     <row r="95" spans="1:5">
       <c r="B95" t="s">
         <v>62</v>
       </c>
       <c r="C95" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="D95" t="s">
         <v>2</v>
@@ -2186,47 +2189,47 @@
         <v>62</v>
       </c>
       <c r="C96" t="s">
+        <v>8</v>
+      </c>
+      <c r="D96" t="s">
+        <v>2</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="B97" t="s">
+        <v>62</v>
+      </c>
+      <c r="C97" t="s">
         <v>25</v>
       </c>
-      <c r="D96" t="s">
-        <v>5</v>
-      </c>
-      <c r="E96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5">
-      <c r="A97" s="2" t="s">
+      <c r="D97" t="s">
+        <v>5</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B97" s="2"/>
-      <c r="C97" s="2"/>
-      <c r="D97" s="2"/>
-      <c r="E97" s="3"/>
-    </row>
-    <row r="99" spans="1:5">
-      <c r="B99" t="s">
-        <v>64</v>
-      </c>
-      <c r="C99" t="s">
-        <v>47</v>
-      </c>
-      <c r="D99" t="s">
-        <v>2</v>
-      </c>
-      <c r="E99">
-        <v>0</v>
-      </c>
+      <c r="B98" s="2"/>
+      <c r="C98" s="2"/>
+      <c r="D98" s="2"/>
+      <c r="E98" s="3"/>
     </row>
     <row r="100" spans="1:5">
       <c r="B100" t="s">
         <v>64</v>
       </c>
       <c r="C100" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="D100" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E100">
         <v>0</v>
@@ -2237,10 +2240,10 @@
         <v>64</v>
       </c>
       <c r="C101" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D101" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="E101">
         <v>0</v>
@@ -2251,10 +2254,10 @@
         <v>64</v>
       </c>
       <c r="C102" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D102" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="E102">
         <v>0</v>
@@ -2265,13 +2268,13 @@
         <v>64</v>
       </c>
       <c r="C103" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D103" t="s">
-        <v>68</v>
+        <v>5</v>
       </c>
       <c r="E103">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -2279,7 +2282,7 @@
         <v>64</v>
       </c>
       <c r="C104" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D104" t="s">
         <v>68</v>
@@ -2293,47 +2296,47 @@
         <v>64</v>
       </c>
       <c r="C105" t="s">
+        <v>69</v>
+      </c>
+      <c r="D105" t="s">
+        <v>68</v>
+      </c>
+      <c r="E105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="B106" t="s">
+        <v>64</v>
+      </c>
+      <c r="C106" t="s">
         <v>70</v>
       </c>
-      <c r="D105" t="s">
-        <v>5</v>
-      </c>
-      <c r="E105">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5">
-      <c r="A106" s="2" t="s">
+      <c r="D106" t="s">
+        <v>5</v>
+      </c>
+      <c r="E106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B106" s="2"/>
-      <c r="C106" s="2"/>
-      <c r="D106" s="2"/>
-      <c r="E106" s="3"/>
-    </row>
-    <row r="108" spans="1:5">
-      <c r="B108" t="s">
-        <v>71</v>
-      </c>
-      <c r="C108" t="s">
-        <v>72</v>
-      </c>
-      <c r="D108" t="s">
-        <v>2</v>
-      </c>
-      <c r="E108">
-        <v>0</v>
-      </c>
+      <c r="B107" s="2"/>
+      <c r="C107" s="2"/>
+      <c r="D107" s="2"/>
+      <c r="E107" s="3"/>
     </row>
     <row r="109" spans="1:5">
       <c r="B109" t="s">
         <v>71</v>
       </c>
       <c r="C109" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="D109" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E109">
         <v>0</v>
@@ -2344,44 +2347,44 @@
         <v>71</v>
       </c>
       <c r="C110" t="s">
+        <v>45</v>
+      </c>
+      <c r="D110" t="s">
+        <v>5</v>
+      </c>
+      <c r="E110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="B111" t="s">
+        <v>71</v>
+      </c>
+      <c r="C111" t="s">
         <v>73</v>
       </c>
-      <c r="D110" t="s">
-        <v>5</v>
-      </c>
-      <c r="E110">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5">
-      <c r="A111" s="2" t="s">
+      <c r="D111" t="s">
+        <v>5</v>
+      </c>
+      <c r="E111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B111" s="2"/>
-      <c r="C111" s="2"/>
-      <c r="D111" s="2"/>
-      <c r="E111" s="3"/>
-    </row>
-    <row r="113" spans="1:5">
-      <c r="B113" t="s">
-        <v>74</v>
-      </c>
-      <c r="C113" t="s">
-        <v>75</v>
-      </c>
-      <c r="D113" t="s">
-        <v>2</v>
-      </c>
-      <c r="E113">
-        <v>0</v>
-      </c>
+      <c r="B112" s="2"/>
+      <c r="C112" s="2"/>
+      <c r="D112" s="2"/>
+      <c r="E112" s="3"/>
     </row>
     <row r="114" spans="1:5">
       <c r="B114" t="s">
         <v>74</v>
       </c>
       <c r="C114" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D114" t="s">
         <v>2</v>
@@ -2395,44 +2398,44 @@
         <v>74</v>
       </c>
       <c r="C115" t="s">
+        <v>76</v>
+      </c>
+      <c r="D115" t="s">
+        <v>2</v>
+      </c>
+      <c r="E115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="B116" t="s">
+        <v>74</v>
+      </c>
+      <c r="C116" t="s">
         <v>25</v>
       </c>
-      <c r="D115" t="s">
-        <v>5</v>
-      </c>
-      <c r="E115">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5">
-      <c r="A116" s="2" t="s">
+      <c r="D116" t="s">
+        <v>5</v>
+      </c>
+      <c r="E116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B116" s="2"/>
-      <c r="C116" s="2"/>
-      <c r="D116" s="2"/>
-      <c r="E116" s="3"/>
-    </row>
-    <row r="118" spans="1:5">
-      <c r="B118" t="s">
-        <v>77</v>
-      </c>
-      <c r="C118" t="s">
-        <v>78</v>
-      </c>
-      <c r="D118" t="s">
-        <v>2</v>
-      </c>
-      <c r="E118">
-        <v>0</v>
-      </c>
+      <c r="B117" s="2"/>
+      <c r="C117" s="2"/>
+      <c r="D117" s="2"/>
+      <c r="E117" s="3"/>
     </row>
     <row r="119" spans="1:5">
       <c r="B119" t="s">
         <v>77</v>
       </c>
       <c r="C119" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D119" t="s">
         <v>2</v>
@@ -2446,7 +2449,7 @@
         <v>77</v>
       </c>
       <c r="C120" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="D120" t="s">
         <v>2</v>
@@ -2460,10 +2463,10 @@
         <v>77</v>
       </c>
       <c r="C121" t="s">
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="D121" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E121">
         <v>0</v>
@@ -2474,44 +2477,44 @@
         <v>77</v>
       </c>
       <c r="C122" t="s">
+        <v>79</v>
+      </c>
+      <c r="D122" t="s">
+        <v>10</v>
+      </c>
+      <c r="E122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="B123" t="s">
+        <v>77</v>
+      </c>
+      <c r="C123" t="s">
         <v>80</v>
       </c>
-      <c r="D122" t="s">
-        <v>5</v>
-      </c>
-      <c r="E122">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5">
-      <c r="A123" s="2" t="s">
+      <c r="D123" t="s">
+        <v>5</v>
+      </c>
+      <c r="E123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B123" s="2"/>
-      <c r="C123" s="2"/>
-      <c r="D123" s="2"/>
-      <c r="E123" s="3"/>
-    </row>
-    <row r="125" spans="1:5">
-      <c r="B125" t="s">
-        <v>81</v>
-      </c>
-      <c r="C125" t="s">
-        <v>82</v>
-      </c>
-      <c r="D125" t="s">
-        <v>2</v>
-      </c>
-      <c r="E125">
-        <v>0</v>
-      </c>
+      <c r="B124" s="2"/>
+      <c r="C124" s="2"/>
+      <c r="D124" s="2"/>
+      <c r="E124" s="3"/>
     </row>
     <row r="126" spans="1:5">
       <c r="B126" t="s">
         <v>81</v>
       </c>
       <c r="C126" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D126" t="s">
         <v>2</v>
@@ -2525,44 +2528,44 @@
         <v>81</v>
       </c>
       <c r="C127" t="s">
+        <v>72</v>
+      </c>
+      <c r="D127" t="s">
+        <v>2</v>
+      </c>
+      <c r="E127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="B128" t="s">
+        <v>81</v>
+      </c>
+      <c r="C128" t="s">
         <v>45</v>
       </c>
-      <c r="D127" t="s">
-        <v>5</v>
-      </c>
-      <c r="E127">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5">
-      <c r="A128" s="2" t="s">
+      <c r="D128" t="s">
+        <v>5</v>
+      </c>
+      <c r="E128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B128" s="2"/>
-      <c r="C128" s="2"/>
-      <c r="D128" s="2"/>
-      <c r="E128" s="3"/>
-    </row>
-    <row r="130" spans="1:5">
-      <c r="B130" t="s">
-        <v>83</v>
-      </c>
-      <c r="C130" t="s">
-        <v>76</v>
-      </c>
-      <c r="D130" t="s">
-        <v>2</v>
-      </c>
-      <c r="E130">
-        <v>0</v>
-      </c>
+      <c r="B129" s="2"/>
+      <c r="C129" s="2"/>
+      <c r="D129" s="2"/>
+      <c r="E129" s="3"/>
     </row>
     <row r="131" spans="1:5">
       <c r="B131" t="s">
         <v>83</v>
       </c>
       <c r="C131" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D131" t="s">
         <v>2</v>
@@ -2576,10 +2579,10 @@
         <v>83</v>
       </c>
       <c r="C132" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="D132" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E132">
         <v>0</v>
@@ -2590,7 +2593,7 @@
         <v>83</v>
       </c>
       <c r="C133" t="s">
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="D133" t="s">
         <v>5</v>
@@ -2604,10 +2607,10 @@
         <v>83</v>
       </c>
       <c r="C134" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
       <c r="D134" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E134">
         <v>0</v>
@@ -2618,10 +2621,10 @@
         <v>83</v>
       </c>
       <c r="C135" t="s">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="D135" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E135">
         <v>0</v>
@@ -2632,44 +2635,44 @@
         <v>83</v>
       </c>
       <c r="C136" t="s">
+        <v>85</v>
+      </c>
+      <c r="D136" t="s">
+        <v>13</v>
+      </c>
+      <c r="E136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
+      <c r="B137" t="s">
+        <v>83</v>
+      </c>
+      <c r="C137" t="s">
         <v>15</v>
       </c>
-      <c r="D136" t="s">
-        <v>2</v>
-      </c>
-      <c r="E136">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5">
-      <c r="A137" s="2" t="s">
+      <c r="D137" t="s">
+        <v>2</v>
+      </c>
+      <c r="E137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
+      <c r="A138" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B137" s="2"/>
-      <c r="C137" s="2"/>
-      <c r="D137" s="2"/>
-      <c r="E137" s="3"/>
-    </row>
-    <row r="139" spans="1:5">
-      <c r="B139" t="s">
-        <v>86</v>
-      </c>
-      <c r="C139" t="s">
-        <v>87</v>
-      </c>
-      <c r="D139" t="s">
-        <v>2</v>
-      </c>
-      <c r="E139">
-        <v>0</v>
-      </c>
+      <c r="B138" s="2"/>
+      <c r="C138" s="2"/>
+      <c r="D138" s="2"/>
+      <c r="E138" s="3"/>
     </row>
     <row r="140" spans="1:5">
       <c r="B140" t="s">
         <v>86</v>
       </c>
       <c r="C140" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D140" t="s">
         <v>2</v>
@@ -2683,7 +2686,7 @@
         <v>86</v>
       </c>
       <c r="C141" t="s">
-        <v>15</v>
+        <v>88</v>
       </c>
       <c r="D141" t="s">
         <v>2</v>
@@ -2697,84 +2700,84 @@
         <v>86</v>
       </c>
       <c r="C142" t="s">
+        <v>15</v>
+      </c>
+      <c r="D142" t="s">
+        <v>2</v>
+      </c>
+      <c r="E142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="B143" t="s">
+        <v>86</v>
+      </c>
+      <c r="C143" t="s">
         <v>89</v>
       </c>
-      <c r="D142" t="s">
+      <c r="D143" t="s">
         <v>10</v>
       </c>
-      <c r="E142">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5">
-      <c r="A143" s="2" t="s">
+      <c r="E143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="A144" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B143" s="2"/>
-      <c r="C143" s="2"/>
-      <c r="D143" s="2"/>
-      <c r="E143" s="3"/>
-    </row>
-    <row r="145" spans="1:5">
-      <c r="B145" t="s">
-        <v>90</v>
-      </c>
-      <c r="C145" t="s">
-        <v>88</v>
-      </c>
-      <c r="D145" t="s">
-        <v>2</v>
-      </c>
-      <c r="E145">
-        <v>0</v>
-      </c>
+      <c r="B144" s="2"/>
+      <c r="C144" s="2"/>
+      <c r="D144" s="2"/>
+      <c r="E144" s="3"/>
     </row>
     <row r="146" spans="1:5">
       <c r="B146" t="s">
         <v>90</v>
       </c>
       <c r="C146" t="s">
+        <v>88</v>
+      </c>
+      <c r="D146" t="s">
+        <v>2</v>
+      </c>
+      <c r="E146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
+      <c r="B147" t="s">
+        <v>90</v>
+      </c>
+      <c r="C147" t="s">
         <v>91</v>
       </c>
-      <c r="D146" t="s">
-        <v>5</v>
-      </c>
-      <c r="E146">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5">
-      <c r="A147" s="2" t="s">
+      <c r="D147" t="s">
+        <v>5</v>
+      </c>
+      <c r="E147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
+      <c r="A148" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B147" s="2"/>
-      <c r="C147" s="2"/>
-      <c r="D147" s="2"/>
-      <c r="E147" s="3"/>
-    </row>
-    <row r="149" spans="1:5">
-      <c r="B149" t="s">
-        <v>92</v>
-      </c>
-      <c r="C149" t="s">
-        <v>93</v>
-      </c>
-      <c r="D149" t="s">
-        <v>2</v>
-      </c>
-      <c r="E149">
-        <v>0</v>
-      </c>
+      <c r="B148" s="2"/>
+      <c r="C148" s="2"/>
+      <c r="D148" s="2"/>
+      <c r="E148" s="3"/>
     </row>
     <row r="150" spans="1:5">
       <c r="B150" t="s">
         <v>92</v>
       </c>
       <c r="C150" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D150" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E150">
         <v>0</v>
@@ -2785,44 +2788,44 @@
         <v>92</v>
       </c>
       <c r="C151" t="s">
+        <v>94</v>
+      </c>
+      <c r="D151" t="s">
+        <v>5</v>
+      </c>
+      <c r="E151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
+      <c r="B152" t="s">
+        <v>92</v>
+      </c>
+      <c r="C152" t="s">
         <v>95</v>
       </c>
-      <c r="D151" t="s">
-        <v>2</v>
-      </c>
-      <c r="E151">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5">
-      <c r="A152" s="2" t="s">
+      <c r="D152" t="s">
+        <v>2</v>
+      </c>
+      <c r="E152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
+      <c r="A153" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B152" s="2"/>
-      <c r="C152" s="2"/>
-      <c r="D152" s="2"/>
-      <c r="E152" s="3"/>
-    </row>
-    <row r="154" spans="1:5">
-      <c r="B154" t="s">
-        <v>96</v>
-      </c>
-      <c r="C154" t="s">
-        <v>97</v>
-      </c>
-      <c r="D154" t="s">
-        <v>2</v>
-      </c>
-      <c r="E154">
-        <v>0</v>
-      </c>
+      <c r="B153" s="2"/>
+      <c r="C153" s="2"/>
+      <c r="D153" s="2"/>
+      <c r="E153" s="3"/>
     </row>
     <row r="155" spans="1:5">
       <c r="B155" t="s">
         <v>96</v>
       </c>
       <c r="C155" t="s">
-        <v>15</v>
+        <v>97</v>
       </c>
       <c r="D155" t="s">
         <v>2</v>
@@ -2836,7 +2839,7 @@
         <v>96</v>
       </c>
       <c r="C156" t="s">
-        <v>98</v>
+        <v>15</v>
       </c>
       <c r="D156" t="s">
         <v>2</v>
@@ -2850,7 +2853,7 @@
         <v>96</v>
       </c>
       <c r="C157" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D157" t="s">
         <v>2</v>
@@ -2864,10 +2867,10 @@
         <v>96</v>
       </c>
       <c r="C158" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D158" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E158">
         <v>0</v>
@@ -2878,118 +2881,118 @@
         <v>96</v>
       </c>
       <c r="C159" t="s">
+        <v>100</v>
+      </c>
+      <c r="D159" t="s">
+        <v>5</v>
+      </c>
+      <c r="E159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5">
+      <c r="B160" t="s">
+        <v>96</v>
+      </c>
+      <c r="C160" t="s">
         <v>95</v>
       </c>
-      <c r="D159" t="s">
-        <v>2</v>
-      </c>
-      <c r="E159">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5">
-      <c r="A160" s="2" t="s">
+      <c r="D160" t="s">
+        <v>2</v>
+      </c>
+      <c r="E160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
+      <c r="A161" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B160" s="2"/>
-      <c r="C160" s="2"/>
-      <c r="D160" s="2"/>
-      <c r="E160" s="3"/>
-    </row>
-    <row r="162" spans="1:5">
-      <c r="B162" t="s">
-        <v>101</v>
-      </c>
-      <c r="C162" t="s">
-        <v>95</v>
-      </c>
-      <c r="D162" t="s">
-        <v>2</v>
-      </c>
-      <c r="E162">
-        <v>0</v>
-      </c>
+      <c r="B161" s="2"/>
+      <c r="C161" s="2"/>
+      <c r="D161" s="2"/>
+      <c r="E161" s="3"/>
     </row>
     <row r="163" spans="1:5">
       <c r="B163" t="s">
         <v>101</v>
       </c>
       <c r="C163" t="s">
+        <v>95</v>
+      </c>
+      <c r="D163" t="s">
+        <v>2</v>
+      </c>
+      <c r="E163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
+      <c r="B164" t="s">
+        <v>101</v>
+      </c>
+      <c r="C164" t="s">
         <v>102</v>
       </c>
-      <c r="D163" t="s">
-        <v>5</v>
-      </c>
-      <c r="E163">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5">
-      <c r="A164" s="2" t="s">
+      <c r="D164" t="s">
+        <v>5</v>
+      </c>
+      <c r="E164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
+      <c r="A165" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B164" s="2"/>
-      <c r="C164" s="2"/>
-      <c r="D164" s="2"/>
-      <c r="E164" s="3"/>
-    </row>
-    <row r="166" spans="1:5">
-      <c r="B166" t="s">
-        <v>103</v>
-      </c>
-      <c r="C166" t="s">
-        <v>98</v>
-      </c>
-      <c r="D166" t="s">
-        <v>2</v>
-      </c>
-      <c r="E166">
-        <v>0</v>
-      </c>
+      <c r="B165" s="2"/>
+      <c r="C165" s="2"/>
+      <c r="D165" s="2"/>
+      <c r="E165" s="3"/>
     </row>
     <row r="167" spans="1:5">
       <c r="B167" t="s">
         <v>103</v>
       </c>
       <c r="C167" t="s">
+        <v>98</v>
+      </c>
+      <c r="D167" t="s">
+        <v>2</v>
+      </c>
+      <c r="E167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
+      <c r="B168" t="s">
+        <v>103</v>
+      </c>
+      <c r="C168" t="s">
         <v>104</v>
       </c>
-      <c r="D167" t="s">
-        <v>5</v>
-      </c>
-      <c r="E167">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5">
-      <c r="A168" s="2" t="s">
+      <c r="D168" t="s">
+        <v>5</v>
+      </c>
+      <c r="E168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
+      <c r="A169" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B168" s="2"/>
-      <c r="C168" s="2"/>
-      <c r="D168" s="2"/>
-      <c r="E168" s="3"/>
-    </row>
-    <row r="170" spans="1:5">
-      <c r="B170" t="s">
-        <v>105</v>
-      </c>
-      <c r="C170" t="s">
-        <v>106</v>
-      </c>
-      <c r="D170" t="s">
-        <v>2</v>
-      </c>
-      <c r="E170">
-        <v>0</v>
-      </c>
+      <c r="B169" s="2"/>
+      <c r="C169" s="2"/>
+      <c r="D169" s="2"/>
+      <c r="E169" s="3"/>
     </row>
     <row r="171" spans="1:5">
       <c r="B171" t="s">
         <v>105</v>
       </c>
       <c r="C171" t="s">
-        <v>15</v>
+        <v>106</v>
       </c>
       <c r="D171" t="s">
         <v>2</v>
@@ -3003,7 +3006,7 @@
         <v>105</v>
       </c>
       <c r="C172" t="s">
-        <v>107</v>
+        <v>15</v>
       </c>
       <c r="D172" t="s">
         <v>2</v>
@@ -3017,44 +3020,44 @@
         <v>105</v>
       </c>
       <c r="C173" t="s">
+        <v>107</v>
+      </c>
+      <c r="D173" t="s">
+        <v>2</v>
+      </c>
+      <c r="E173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5">
+      <c r="B174" t="s">
+        <v>105</v>
+      </c>
+      <c r="C174" t="s">
         <v>156</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D174" t="s">
         <v>13</v>
       </c>
-      <c r="E173">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5">
-      <c r="A174" s="2" t="s">
+      <c r="E174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
+      <c r="A175" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B174" s="2"/>
-      <c r="C174" s="2"/>
-      <c r="D174" s="2"/>
-      <c r="E174" s="3"/>
-    </row>
-    <row r="176" spans="1:5">
-      <c r="B176" t="s">
-        <v>108</v>
-      </c>
-      <c r="C176" t="s">
-        <v>109</v>
-      </c>
-      <c r="D176" t="s">
-        <v>2</v>
-      </c>
-      <c r="E176">
-        <v>0</v>
-      </c>
+      <c r="B175" s="2"/>
+      <c r="C175" s="2"/>
+      <c r="D175" s="2"/>
+      <c r="E175" s="3"/>
     </row>
     <row r="177" spans="1:5">
       <c r="B177" t="s">
         <v>108</v>
       </c>
       <c r="C177" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D177" t="s">
         <v>2</v>
@@ -3068,7 +3071,7 @@
         <v>108</v>
       </c>
       <c r="C178" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D178" t="s">
         <v>2</v>
@@ -3082,10 +3085,10 @@
         <v>108</v>
       </c>
       <c r="C179" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D179" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E179">
         <v>0</v>
@@ -3096,81 +3099,81 @@
         <v>108</v>
       </c>
       <c r="C180" t="s">
+        <v>112</v>
+      </c>
+      <c r="D180" t="s">
+        <v>5</v>
+      </c>
+      <c r="E180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
+      <c r="B181" t="s">
+        <v>108</v>
+      </c>
+      <c r="C181" t="s">
         <v>113</v>
       </c>
-      <c r="D180" t="s">
+      <c r="D181" t="s">
         <v>114</v>
       </c>
-      <c r="E180">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5">
-      <c r="A181" s="2" t="s">
+      <c r="E181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5">
+      <c r="A182" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B181" s="2"/>
-      <c r="C181" s="2"/>
-      <c r="D181" s="2"/>
-      <c r="E181" s="3"/>
-    </row>
-    <row r="183" spans="1:5">
-      <c r="B183" t="s">
-        <v>115</v>
-      </c>
-      <c r="C183" t="s">
-        <v>17</v>
-      </c>
-      <c r="D183" t="s">
-        <v>2</v>
-      </c>
-      <c r="E183">
-        <v>0</v>
-      </c>
+      <c r="B182" s="2"/>
+      <c r="C182" s="2"/>
+      <c r="D182" s="2"/>
+      <c r="E182" s="3"/>
     </row>
     <row r="184" spans="1:5">
       <c r="B184" t="s">
         <v>115</v>
       </c>
       <c r="C184" t="s">
+        <v>17</v>
+      </c>
+      <c r="D184" t="s">
+        <v>2</v>
+      </c>
+      <c r="E184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5">
+      <c r="B185" t="s">
+        <v>115</v>
+      </c>
+      <c r="C185" t="s">
         <v>116</v>
       </c>
-      <c r="D184" t="s">
-        <v>2</v>
-      </c>
-      <c r="E184">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5">
-      <c r="A185" s="2" t="s">
+      <c r="D185" t="s">
+        <v>2</v>
+      </c>
+      <c r="E185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5">
+      <c r="A186" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B185" s="2"/>
-      <c r="C185" s="2"/>
-      <c r="D185" s="2"/>
-      <c r="E185" s="3"/>
-    </row>
-    <row r="187" spans="1:5">
-      <c r="B187" t="s">
-        <v>117</v>
-      </c>
-      <c r="C187" t="s">
-        <v>118</v>
-      </c>
-      <c r="D187" t="s">
-        <v>2</v>
-      </c>
-      <c r="E187">
-        <v>0</v>
-      </c>
+      <c r="B186" s="2"/>
+      <c r="C186" s="2"/>
+      <c r="D186" s="2"/>
+      <c r="E186" s="3"/>
     </row>
     <row r="188" spans="1:5">
       <c r="B188" t="s">
         <v>117</v>
       </c>
       <c r="C188" t="s">
-        <v>8</v>
+        <v>118</v>
       </c>
       <c r="D188" t="s">
         <v>2</v>
@@ -3184,7 +3187,7 @@
         <v>117</v>
       </c>
       <c r="C189" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D189" t="s">
         <v>2</v>
@@ -3198,10 +3201,10 @@
         <v>117</v>
       </c>
       <c r="C190" t="s">
-        <v>119</v>
+        <v>15</v>
       </c>
       <c r="D190" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E190">
         <v>0</v>
@@ -3212,58 +3215,58 @@
         <v>117</v>
       </c>
       <c r="C191" t="s">
+        <v>119</v>
+      </c>
+      <c r="D191" t="s">
+        <v>5</v>
+      </c>
+      <c r="E191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5">
+      <c r="B192" t="s">
+        <v>117</v>
+      </c>
+      <c r="C192" t="s">
         <v>120</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D192" t="s">
         <v>10</v>
       </c>
-      <c r="E191">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5">
-      <c r="A192" s="2" t="s">
+      <c r="E192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5">
+      <c r="A193" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B192" s="2"/>
-      <c r="C192" s="2"/>
-      <c r="D192" s="2"/>
-      <c r="E192" s="3"/>
-    </row>
-    <row r="194" spans="2:5">
-      <c r="B194" t="s">
-        <v>121</v>
-      </c>
-      <c r="C194" t="s">
-        <v>15</v>
-      </c>
-      <c r="D194" t="s">
-        <v>2</v>
-      </c>
-      <c r="E194">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="195" spans="2:5">
+      <c r="B193" s="2"/>
+      <c r="C193" s="2"/>
+      <c r="D193" s="2"/>
+      <c r="E193" s="3"/>
+    </row>
+    <row r="195" spans="1:5">
       <c r="B195" t="s">
         <v>121</v>
       </c>
       <c r="C195" t="s">
-        <v>122</v>
+        <v>15</v>
       </c>
       <c r="D195" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E195">
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="2:5">
+    <row r="196" spans="1:5">
       <c r="B196" t="s">
         <v>121</v>
       </c>
       <c r="C196" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D196" t="s">
         <v>5</v>
@@ -3272,40 +3275,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="2:5">
+    <row r="197" spans="1:5">
       <c r="B197" t="s">
         <v>121</v>
       </c>
       <c r="C197" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D197" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E197">
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="2:5">
+    <row r="198" spans="1:5">
       <c r="B198" t="s">
         <v>121</v>
       </c>
       <c r="C198" t="s">
-        <v>45</v>
+        <v>124</v>
       </c>
       <c r="D198" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E198">
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="2:5">
+    <row r="199" spans="1:5">
       <c r="B199" t="s">
         <v>121</v>
       </c>
       <c r="C199" t="s">
-        <v>125</v>
+        <v>45</v>
       </c>
       <c r="D199" t="s">
         <v>5</v>
@@ -3314,96 +3317,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="2:5">
+    <row r="200" spans="1:5">
       <c r="B200" t="s">
         <v>121</v>
       </c>
       <c r="C200" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D200" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E200">
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="2:5">
+    <row r="201" spans="1:5">
       <c r="B201" t="s">
         <v>121</v>
       </c>
       <c r="C201" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D201" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E201">
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="2:5">
+    <row r="202" spans="1:5">
       <c r="B202" t="s">
         <v>121</v>
       </c>
       <c r="C202" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D202" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E202">
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="2:5">
+    <row r="203" spans="1:5">
       <c r="B203" t="s">
         <v>121</v>
       </c>
       <c r="C203" t="s">
-        <v>65</v>
+        <v>128</v>
       </c>
       <c r="D203" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E203">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="204" spans="2:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5">
       <c r="B204" t="s">
         <v>121</v>
       </c>
       <c r="C204" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
       <c r="D204" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="E204">
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="2:5">
+    <row r="205" spans="1:5">
       <c r="B205" t="s">
         <v>121</v>
       </c>
       <c r="C205" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D205" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="E205">
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="2:5">
+    <row r="206" spans="1:5">
       <c r="B206" t="s">
         <v>121</v>
       </c>
       <c r="C206" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D206" t="s">
         <v>5</v>
@@ -3412,26 +3415,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="2:5">
+    <row r="207" spans="1:5">
       <c r="B207" t="s">
         <v>121</v>
       </c>
       <c r="C207" t="s">
-        <v>12</v>
+        <v>131</v>
       </c>
       <c r="D207" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E207">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="208" spans="2:5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5">
       <c r="B208" t="s">
         <v>121</v>
       </c>
       <c r="C208" t="s">
-        <v>132</v>
+        <v>12</v>
       </c>
       <c r="D208" t="s">
         <v>13</v>
@@ -3445,13 +3448,13 @@
         <v>121</v>
       </c>
       <c r="C209" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D209" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E209">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="210" spans="1:5">
@@ -3459,7 +3462,7 @@
         <v>121</v>
       </c>
       <c r="C210" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D210" t="s">
         <v>5</v>
@@ -3469,34 +3472,34 @@
       </c>
     </row>
     <row r="211" spans="1:5">
-      <c r="A211" s="2" t="s">
+      <c r="B211" t="s">
+        <v>121</v>
+      </c>
+      <c r="C211" t="s">
+        <v>134</v>
+      </c>
+      <c r="D211" t="s">
+        <v>5</v>
+      </c>
+      <c r="E211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5">
+      <c r="A212" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B211" s="2"/>
-      <c r="C211" s="2"/>
-      <c r="D211" s="2"/>
-      <c r="E211" s="3"/>
-    </row>
-    <row r="213" spans="1:5">
-      <c r="B213" t="s">
-        <v>135</v>
-      </c>
-      <c r="C213" t="s">
-        <v>136</v>
-      </c>
-      <c r="D213" t="s">
-        <v>2</v>
-      </c>
-      <c r="E213">
-        <v>0</v>
-      </c>
+      <c r="B212" s="2"/>
+      <c r="C212" s="2"/>
+      <c r="D212" s="2"/>
+      <c r="E212" s="3"/>
     </row>
     <row r="214" spans="1:5">
       <c r="B214" t="s">
         <v>135</v>
       </c>
       <c r="C214" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="D214" t="s">
         <v>2</v>
@@ -3510,44 +3513,44 @@
         <v>135</v>
       </c>
       <c r="C215" t="s">
+        <v>15</v>
+      </c>
+      <c r="D215" t="s">
+        <v>2</v>
+      </c>
+      <c r="E215">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5">
+      <c r="B216" t="s">
+        <v>135</v>
+      </c>
+      <c r="C216" t="s">
         <v>17</v>
       </c>
-      <c r="D215" t="s">
-        <v>2</v>
-      </c>
-      <c r="E215">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5">
-      <c r="A216" s="2" t="s">
+      <c r="D216" t="s">
+        <v>2</v>
+      </c>
+      <c r="E216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5">
+      <c r="A217" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B216" s="2"/>
-      <c r="C216" s="2"/>
-      <c r="D216" s="2"/>
-      <c r="E216" s="3"/>
-    </row>
-    <row r="218" spans="1:5">
-      <c r="B218" t="s">
-        <v>137</v>
-      </c>
-      <c r="C218" t="s">
-        <v>138</v>
-      </c>
-      <c r="D218" t="s">
-        <v>2</v>
-      </c>
-      <c r="E218">
-        <v>0</v>
-      </c>
+      <c r="B217" s="2"/>
+      <c r="C217" s="2"/>
+      <c r="D217" s="2"/>
+      <c r="E217" s="3"/>
     </row>
     <row r="219" spans="1:5">
       <c r="B219" t="s">
         <v>137</v>
       </c>
       <c r="C219" t="s">
-        <v>8</v>
+        <v>138</v>
       </c>
       <c r="D219" t="s">
         <v>2</v>
@@ -3561,7 +3564,7 @@
         <v>137</v>
       </c>
       <c r="C220" t="s">
-        <v>139</v>
+        <v>8</v>
       </c>
       <c r="D220" t="s">
         <v>2</v>
@@ -3575,7 +3578,7 @@
         <v>137</v>
       </c>
       <c r="C221" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D221" t="s">
         <v>2</v>
@@ -3589,10 +3592,10 @@
         <v>137</v>
       </c>
       <c r="C222" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D222" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E222">
         <v>0</v>
@@ -3603,44 +3606,44 @@
         <v>137</v>
       </c>
       <c r="C223" t="s">
+        <v>141</v>
+      </c>
+      <c r="D223" t="s">
+        <v>10</v>
+      </c>
+      <c r="E223">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5">
+      <c r="B224" t="s">
+        <v>137</v>
+      </c>
+      <c r="C224" t="s">
         <v>142</v>
       </c>
-      <c r="D223" t="s">
+      <c r="D224" t="s">
         <v>13</v>
       </c>
-      <c r="E223">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="224" spans="1:5">
-      <c r="A224" s="2" t="s">
+      <c r="E224">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5">
+      <c r="A225" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B224" s="2"/>
-      <c r="C224" s="2"/>
-      <c r="D224" s="2"/>
-      <c r="E224" s="3"/>
-    </row>
-    <row r="226" spans="1:5">
-      <c r="B226" t="s">
-        <v>143</v>
-      </c>
-      <c r="C226" t="s">
-        <v>144</v>
-      </c>
-      <c r="D226" t="s">
-        <v>2</v>
-      </c>
-      <c r="E226">
-        <v>0</v>
-      </c>
+      <c r="B225" s="2"/>
+      <c r="C225" s="2"/>
+      <c r="D225" s="2"/>
+      <c r="E225" s="3"/>
     </row>
     <row r="227" spans="1:5">
       <c r="B227" t="s">
         <v>143</v>
       </c>
       <c r="C227" t="s">
-        <v>8</v>
+        <v>144</v>
       </c>
       <c r="D227" t="s">
         <v>2</v>
@@ -3654,7 +3657,7 @@
         <v>143</v>
       </c>
       <c r="C228" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D228" t="s">
         <v>2</v>
@@ -3668,10 +3671,10 @@
         <v>143</v>
       </c>
       <c r="C229" t="s">
-        <v>112</v>
+        <v>15</v>
       </c>
       <c r="D229" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E229">
         <v>0</v>
@@ -3682,13 +3685,13 @@
         <v>143</v>
       </c>
       <c r="C230" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D230" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="E230">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="231" spans="1:5">
@@ -3696,44 +3699,44 @@
         <v>143</v>
       </c>
       <c r="C231" t="s">
+        <v>113</v>
+      </c>
+      <c r="D231" t="s">
+        <v>31</v>
+      </c>
+      <c r="E231">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5">
+      <c r="B232" t="s">
+        <v>143</v>
+      </c>
+      <c r="C232" t="s">
         <v>145</v>
       </c>
-      <c r="D231" t="s">
+      <c r="D232" t="s">
         <v>10</v>
       </c>
-      <c r="E231">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="232" spans="1:5">
-      <c r="A232" s="2" t="s">
+      <c r="E232">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5">
+      <c r="A233" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B232" s="2"/>
-      <c r="C232" s="2"/>
-      <c r="D232" s="2"/>
-      <c r="E232" s="3"/>
-    </row>
-    <row r="234" spans="1:5">
-      <c r="B234" t="s">
-        <v>146</v>
-      </c>
-      <c r="C234" t="s">
-        <v>147</v>
-      </c>
-      <c r="D234" t="s">
-        <v>2</v>
-      </c>
-      <c r="E234">
-        <v>0</v>
-      </c>
+      <c r="B233" s="2"/>
+      <c r="C233" s="2"/>
+      <c r="D233" s="2"/>
+      <c r="E233" s="3"/>
     </row>
     <row r="235" spans="1:5">
       <c r="B235" t="s">
         <v>146</v>
       </c>
       <c r="C235" t="s">
-        <v>8</v>
+        <v>147</v>
       </c>
       <c r="D235" t="s">
         <v>2</v>
@@ -3747,7 +3750,7 @@
         <v>146</v>
       </c>
       <c r="C236" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D236" t="s">
         <v>2</v>
@@ -3761,10 +3764,10 @@
         <v>146</v>
       </c>
       <c r="C237" t="s">
-        <v>124</v>
+        <v>15</v>
       </c>
       <c r="D237" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E237">
         <v>0</v>
@@ -3775,13 +3778,13 @@
         <v>146</v>
       </c>
       <c r="C238" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="D238" t="s">
         <v>10</v>
       </c>
       <c r="E238">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="239" spans="1:5">
@@ -3789,23 +3792,37 @@
         <v>146</v>
       </c>
       <c r="C239" t="s">
+        <v>148</v>
+      </c>
+      <c r="D239" t="s">
+        <v>10</v>
+      </c>
+      <c r="E239">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5">
+      <c r="B240" t="s">
+        <v>146</v>
+      </c>
+      <c r="C240" t="s">
         <v>149</v>
       </c>
-      <c r="D239" t="s">
+      <c r="D240" t="s">
         <v>13</v>
       </c>
-      <c r="E239">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="240" spans="1:5">
-      <c r="A240" s="2" t="s">
+      <c r="E240">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5">
+      <c r="A241" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B240" s="2"/>
-      <c r="C240" s="2"/>
-      <c r="D240" s="2"/>
-      <c r="E240" s="3"/>
+      <c r="B241" s="2"/>
+      <c r="C241" s="2"/>
+      <c r="D241" s="2"/>
+      <c r="E241" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>